<commit_message>
Cambios en la Demanda
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_DemProj_ELC.xlsx
+++ b/SuppXLS/Scen_DemProj_ELC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Caso_Base_Junio_VEDA\CasoBase_Junio_Simulacion\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BEF6D7-4E69-4C48-B023-C0314BC31816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA24B88C-7DEE-47A9-AF09-4CC0704A3B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -866,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
@@ -945,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1006,13 +1006,13 @@
       </c>
       <c r="F4" s="12">
         <f>BY_Data!$H$4*(1+$J$4)^(E4-2005)</f>
-        <v>10838.880000000001</v>
+        <v>10734.66</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="9">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="F5" s="12">
         <f>BY_Data!$H$4*(1+$J$4)^(E5-2005)</f>
-        <v>12679.956548812803</v>
+        <v>12081.954402354599</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="F6" s="12">
         <f>BY_Data!$H$4*(1+$J$4)^(E6-2005)</f>
-        <v>15427.105937418988</v>
+        <v>14006.296505524437</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="F7" s="12">
         <f>BY_Data!$H$4*(1+$J$4)^(E7-2005)</f>
-        <v>18769.433214393088</v>
+        <v>16237.136415813167</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>

</xml_diff>